<commit_message>
updated data with political affiliation, sex and info
</commit_message>
<xml_diff>
--- a/Stiftungsrat.xlsx
+++ b/Stiftungsrat.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="89">
   <si>
     <t>Stiftungsrat</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Geschäftsführerin Wiener Frauenhäuser</t>
+  </si>
+  <si>
+    <t>Generalsekretär Sportunion</t>
+  </si>
+  <si>
+    <t>Management Staatsdruckerei</t>
   </si>
 </sst>
 </file>
@@ -630,16 +636,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="48.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
@@ -661,7 +668,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -712,7 +719,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>26</v>
       </c>
@@ -729,7 +736,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -746,7 +753,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -763,7 +770,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -780,7 +787,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -794,7 +801,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -811,7 +818,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -822,7 +829,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -839,7 +846,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -856,7 +863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -873,7 +880,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -907,7 +914,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -924,7 +931,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -941,18 +948,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>31</v>
       </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
       <c r="F19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -969,7 +979,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -986,7 +996,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>36</v>
       </c>
@@ -1003,7 +1013,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>40</v>
       </c>
@@ -1054,7 +1064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>42</v>
       </c>
@@ -1072,11 +1082,17 @@
       <c r="C27" t="s">
         <v>43</v>
       </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -1124,7 +1140,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>50</v>
       </c>
@@ -1141,7 +1157,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>21</v>
       </c>
@@ -1158,7 +1174,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>21</v>
       </c>
@@ -1175,7 +1191,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>21</v>
       </c>
@@ -1199,11 +1215,17 @@
       <c r="C35" t="s">
         <v>54</v>
       </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="F35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1237,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B36"/>
+  <autoFilter ref="B1:B36">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Bundesregierung"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>